<commit_message>
start week 1 worksheet
</commit_message>
<xml_diff>
--- a/Week 1/Lab1_BestPractices.xlsx
+++ b/Week 1/Lab1_BestPractices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stark State\Spring 2020\WDD229 Adv Web Design\Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\wdd229\Week 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC2E32C-6324-4946-A159-C3E0B3201AD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE2B8EE-1C7E-4238-BD90-303151DA53A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="2235" windowWidth="13125" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="13125" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="89">
   <si>
     <t>Page Layout</t>
   </si>
@@ -269,6 +269,24 @@
   </si>
   <si>
     <t>Answer here</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>no update information</t>
+  </si>
+  <si>
+    <t>contrast ratio of 6.23</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>no '&lt;meta name="viewport"&gt;' tag found</t>
   </si>
 </sst>
 </file>
@@ -696,8 +714,8 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,71 +747,122 @@
       <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="B4" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="B7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="B8" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="B9" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="10" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="11" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="B11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="12" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B12" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="14" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B14" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="16" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B16" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
@@ -809,6 +878,9 @@
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="B19" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
@@ -819,11 +891,17 @@
       <c r="A21" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="B21" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="B22" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -838,6 +916,9 @@
     <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>